<commit_message>
a big catch up commit
</commit_message>
<xml_diff>
--- a/tables/TableX_mgmt_scenarios.xlsx
+++ b/tables/TableX_mgmt_scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/dungeness/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98754BB0-3648-D047-8544-2651CA83E610}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9C244C-525F-764C-A3C5-557B85494229}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{55D2B262-C7B5-5648-8148-68D5EF3DDDE1}"/>
+    <workbookView xWindow="620" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{55D2B262-C7B5-5648-8148-68D5EF3DDDE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="2" r:id="rId1"/>
@@ -166,9 +166,6 @@
     <t>Ad-hoc sampling</t>
   </si>
   <si>
-    <t>More locations (more samples?)</t>
-  </si>
-  <si>
     <t>WE-Settle</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>Original RAMP guidelines</t>
+  </si>
+  <si>
+    <t>More locations</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A1DE32-064F-3347-A13F-C83622F1F548}">
   <dimension ref="A2:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+    <sheetView zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -801,7 +801,7 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -809,7 +809,7 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
@@ -825,7 +825,7 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
@@ -836,7 +836,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
         <v>16</v>
@@ -851,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3BCF9D-76AF-6349-B360-573DE52E4DBD}">
   <dimension ref="B2:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="B2:D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,7 +888,7 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>